<commit_message>
implement import ds lop
</commit_message>
<xml_diff>
--- a/mockupData_python/dataTempalte.xlsx
+++ b/mockupData_python/dataTempalte.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phong\OneDrive\Máy tính\FakeDataStudent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phong\OneDrive\Máy tính\datn\git\datn\mockupData_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBBABC2-A301-4F5C-9E25-D8104E0BC23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDE110F-F9F8-4ED1-AEBB-93045785E41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>STT</t>
   </si>
@@ -124,72 +124,6 @@
     <t>07/02/1976</t>
   </si>
   <si>
-    <t>Lê Văn Việt</t>
-  </si>
-  <si>
-    <t>08/02/2002</t>
-  </si>
-  <si>
-    <t>Nam</t>
-  </si>
-  <si>
-    <t>Tày</t>
-  </si>
-  <si>
-    <t>0329743466</t>
-  </si>
-  <si>
-    <t>HCM</t>
-  </si>
-  <si>
-    <t>Lê Văn Nghĩa</t>
-  </si>
-  <si>
-    <t>08/02/1966</t>
-  </si>
-  <si>
-    <t>0329743469</t>
-  </si>
-  <si>
-    <t>Đoàn Thu Trang</t>
-  </si>
-  <si>
-    <t>13/09/1970</t>
-  </si>
-  <si>
-    <t>0329743468</t>
-  </si>
-  <si>
-    <t>Nguyễn Hoài Lâm</t>
-  </si>
-  <si>
-    <t>21/06/2003</t>
-  </si>
-  <si>
-    <t>21/09/2024</t>
-  </si>
-  <si>
-    <t>0329347411</t>
-  </si>
-  <si>
-    <t>Hà Nội</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Nguyễn Văn Ba</t>
-  </si>
-  <si>
-    <t>21/07/1960</t>
-  </si>
-  <si>
-    <t>0329347412</t>
-  </si>
-  <si>
-    <t>Nông dân</t>
-  </si>
-  <si>
     <t>Nghề nghiệp cha</t>
   </si>
   <si>
@@ -208,10 +142,22 @@
     <t>Họ tên mẹ</t>
   </si>
   <si>
-    <t>Ông bà</t>
-  </si>
-  <si>
-    <t>Lê Văn Vinh</t>
+    <t>Năm học</t>
+  </si>
+  <si>
+    <t>Khối</t>
+  </si>
+  <si>
+    <t>Lớp</t>
+  </si>
+  <si>
+    <t>2024-2025</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>1A2</t>
   </si>
 </sst>
 </file>
@@ -588,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -620,9 +566,12 @@
     <col min="23" max="23" width="20" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="23.125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -663,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="O1" t="s">
         <v>13</v>
@@ -672,10 +621,10 @@
         <v>14</v>
       </c>
       <c r="Q1" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="R1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="S1" t="s">
         <v>15</v>
@@ -684,10 +633,10 @@
         <v>16</v>
       </c>
       <c r="U1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="V1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="W1" t="s">
         <v>17</v>
@@ -696,10 +645,19 @@
         <v>18</v>
       </c>
       <c r="Y1" t="s">
-        <v>59</v>
+        <v>37</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -760,250 +718,20 @@
       <c r="U2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" t="s">
-        <v>40</v>
-      </c>
-      <c r="O3" t="s">
-        <v>41</v>
-      </c>
-      <c r="P3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="Z2" t="s">
         <v>43</v>
       </c>
-      <c r="S3" t="s">
+      <c r="AA2" t="s">
         <v>44</v>
       </c>
-      <c r="T3" t="s">
+      <c r="AB2" t="s">
         <v>45</v>
-      </c>
-      <c r="U3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" t="s">
-        <v>62</v>
-      </c>
-      <c r="N4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>51</v>
-      </c>
-      <c r="R4" t="s">
-        <v>51</v>
-      </c>
-      <c r="S4" t="s">
-        <v>51</v>
-      </c>
-      <c r="T4" t="s">
-        <v>51</v>
-      </c>
-      <c r="U4" t="s">
-        <v>51</v>
-      </c>
-      <c r="V4" t="s">
-        <v>52</v>
-      </c>
-      <c r="W4" t="s">
-        <v>53</v>
-      </c>
-      <c r="X4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5">
-        <v>329743468</v>
-      </c>
-      <c r="I5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" t="s">
-        <v>40</v>
-      </c>
-      <c r="O5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P5" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>31</v>
-      </c>
-      <c r="R5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" t="s">
-        <v>28</v>
-      </c>
-      <c r="R6" t="s">
-        <v>43</v>
-      </c>
-      <c r="S6" t="s">
-        <v>44</v>
-      </c>
-      <c r="T6" t="s">
-        <v>45</v>
-      </c>
-      <c r="U6" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2:A4 A1:M1 S1:T1 W1:X1 O1:P1 C2:Y3 C4:L4 N4:Y4" numberStoredAsText="1"/>
+    <ignoredError sqref="A2 A1:M1 S1:T1 W1:X1 O1:P1 C2:Y2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update chức năng thêm lớp mới
</commit_message>
<xml_diff>
--- a/mockupData_python/dataTempalte.xlsx
+++ b/mockupData_python/dataTempalte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phong\OneDrive\Máy tính\datn\git\datn\mockupData_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21562DF0-12CF-4B2B-B40B-F42CA5CED8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF4BE24-1997-4FEE-AC84-54499B9A083F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1A1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Mã số học sinh</t>
-  </si>
-  <si>
     <t>Giới tính</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>Địa chỉ</t>
   </si>
   <si>
-    <t>Trạng thái</t>
-  </si>
-  <si>
     <t>Cha</t>
   </si>
   <si>
@@ -100,13 +94,13 @@
     <t>Lớp</t>
   </si>
   <si>
-    <t>Fist Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>Năm sinh</t>
+  </si>
+  <si>
+    <t>Họ</t>
+  </si>
+  <si>
+    <t>Tên</t>
   </si>
 </sst>
 </file>
@@ -483,137 +477,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Z1" t="s">
         <v>14</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AA1" t="s">
         <v>18</v>
-      </c>
-      <c r="W1" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="F1:N1 T1:U1 X1:Y1 P1:Q1 A1:B1" numberStoredAsText="1"/>
+    <ignoredError sqref="H1:L1 U1:V1 Y1:Z1 Q1:R1 M1:O1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update chức năng thêm lớp mới (#10)
Co-authored-by: LeQuocPhong2k2 <phonglehn2002@gmai.com>
</commit_message>
<xml_diff>
--- a/mockupData_python/dataTempalte.xlsx
+++ b/mockupData_python/dataTempalte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phong\OneDrive\Máy tính\datn\git\datn\mockupData_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21562DF0-12CF-4B2B-B40B-F42CA5CED8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF4BE24-1997-4FEE-AC84-54499B9A083F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1A1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Mã số học sinh</t>
-  </si>
-  <si>
     <t>Giới tính</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>Địa chỉ</t>
   </si>
   <si>
-    <t>Trạng thái</t>
-  </si>
-  <si>
     <t>Cha</t>
   </si>
   <si>
@@ -100,13 +94,13 @@
     <t>Lớp</t>
   </si>
   <si>
-    <t>Fist Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>Năm sinh</t>
+  </si>
+  <si>
+    <t>Họ</t>
+  </si>
+  <si>
+    <t>Tên</t>
   </si>
 </sst>
 </file>
@@ -483,137 +477,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Z1" t="s">
         <v>14</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AA1" t="s">
         <v>18</v>
-      </c>
-      <c r="W1" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="F1:N1 T1:U1 X1:Y1 P1:Q1 A1:B1" numberStoredAsText="1"/>
+    <ignoredError sqref="H1:L1 U1:V1 Y1:Z1 Q1:R1 M1:O1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>